<commit_message>
Added more perverse rewards to training agenda.
</commit_message>
<xml_diff>
--- a/data/c_vs_random.xlsx
+++ b/data/c_vs_random.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="COIN vs. random" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COIN vs. random" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Tested models vs. randomness
</commit_message>
<xml_diff>
--- a/data/c_vs_random.xlsx
+++ b/data/c_vs_random.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COIN vs. random" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="COIN vs. random" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,266 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="C2" t="n">
+        <v>31.548</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="C3" t="n">
+        <v>31.427</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="C4" t="n">
+        <v>31.772</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="C5" t="n">
+        <v>31.441</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>31.457</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>94</v>
+      </c>
+      <c r="C7" t="n">
+        <v>31.557</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>96.2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>31.352</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>96.2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>31.678</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>31.77</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>31.732</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>31.338</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>94.7</v>
+      </c>
+      <c r="C13" t="n">
+        <v>31.532</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>96.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>31.591</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>96.3</v>
+      </c>
+      <c r="C15" t="n">
+        <v>31.199</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="C16" t="n">
+        <v>31.785</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>94.8</v>
+      </c>
+      <c r="C17" t="n">
+        <v>31.35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="C18" t="n">
+        <v>31.44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="C19" t="n">
+        <v>31.396</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>31.333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="C21" t="n">
+        <v>31.362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>